<commit_message>
Text formats and template updated
</commit_message>
<xml_diff>
--- a/Square_ExtractData_CreateTable/Template/Square_Excel_Template.xlsx
+++ b/Square_ExtractData_CreateTable/Template/Square_Excel_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\AUTOCAD\01_Repo\Square_ExtractData_CreateTable\Square_ExtractData_CreateTable\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E9179A-72A7-454F-8134-0388A7BE39A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5F55BA-3DAB-4A4E-A6B3-26E549015C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DF3F688B-7FB6-4411-A5E2-7927D76E8A1F}"/>
   </bookViews>
@@ -63,16 +63,16 @@
     <t>Plot Number</t>
   </si>
   <si>
-    <t>Information</t>
-  </si>
-  <si>
     <t>Areas</t>
   </si>
   <si>
     <t>Sizes</t>
   </si>
   <si>
-    <t>Note: This report is generated by a computer system and should be cross-verified on site for accuracy</t>
+    <t>Note: This report is generated by a computer system and should be cross-verified before registration</t>
+  </si>
+  <si>
+    <t>Boundaries</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A2:M92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J4" sqref="J4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,7 +550,7 @@
   <sheetData>
     <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -568,19 +568,19 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="10"/>
       <c r="I4" s="4"/>
       <c r="J4" s="8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>

</xml_diff>

<commit_message>
template updated to fix column width in east and north
</commit_message>
<xml_diff>
--- a/Square_ExtractData_CreateTable/Template/Square_Excel_Template.xlsx
+++ b/Square_ExtractData_CreateTable/Template/Square_Excel_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Personal\AUTOCAD\01_Repo\Square_ExtractData_CreateTable\Square_ExtractData_CreateTable\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5F55BA-3DAB-4A4E-A6B3-26E549015C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7C31B8-F353-4437-BFFA-CA462FBB4944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DF3F688B-7FB6-4411-A5E2-7927D76E8A1F}"/>
   </bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A2:M92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:M4"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,10 +542,10 @@
     <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="38.77734375" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
     <col min="11" max="11" width="12.5546875" customWidth="1"/>
     <col min="12" max="12" width="13.77734375" customWidth="1"/>
-    <col min="13" max="13" width="12.109375" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>